<commit_message>
GW: Updated data; Started presentation and write-up
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -3173,8 +3173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AD45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3294,27 +3294,27 @@
         <v>0.41299999999999998</v>
       </c>
       <c r="I5" s="2">
-        <f>Y16+C5</f>
+        <f t="shared" ref="I5:I34" si="0">Y16+C5</f>
         <v>2.0999999999999998E-2</v>
       </c>
       <c r="J5" s="3">
-        <f>Z16+D5</f>
+        <f t="shared" ref="J5:J34" si="1">Z16+D5</f>
         <v>3.9E-2</v>
       </c>
       <c r="K5" s="3">
-        <f t="shared" ref="K5:N5" si="0">AA16+E5</f>
+        <f t="shared" ref="K5:N5" si="2">AA16+E5</f>
         <v>0.11199999999999999</v>
       </c>
       <c r="L5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="M5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.5680000000000001</v>
       </c>
       <c r="N5" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10.649000000000001</v>
       </c>
       <c r="Q5" t="s">
@@ -3348,27 +3348,27 @@
         <v>0.78</v>
       </c>
       <c r="I6" s="5">
-        <f>Y17+C6</f>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="J6" s="6">
-        <f>Z17+D6</f>
+        <f t="shared" si="1"/>
         <v>0.77700000000000002</v>
       </c>
       <c r="K6" s="6">
-        <f t="shared" ref="K6:K34" si="1">AA17+E6</f>
+        <f t="shared" ref="K6:K34" si="3">AA17+E6</f>
         <v>0.215</v>
       </c>
       <c r="L6" s="6">
-        <f t="shared" ref="L6:L34" si="2">AB17+F6</f>
+        <f t="shared" ref="L6:L34" si="4">AB17+F6</f>
         <v>0.19600000000000001</v>
       </c>
       <c r="M6" s="6">
-        <f t="shared" ref="M6:M34" si="3">AC17+G6</f>
+        <f t="shared" ref="M6:M34" si="5">AC17+G6</f>
         <v>2.4430000000000001</v>
       </c>
       <c r="N6" s="7">
-        <f t="shared" ref="N6:N34" si="4">AD17+H6</f>
+        <f t="shared" ref="N6:N34" si="6">AD17+H6</f>
         <v>12.955</v>
       </c>
       <c r="Q6" t="s">
@@ -3402,27 +3402,27 @@
         <v>1.0920000000000001</v>
       </c>
       <c r="I7" s="5">
-        <f>Y18+C7</f>
+        <f t="shared" si="0"/>
         <v>35.177</v>
       </c>
       <c r="J7" s="6">
-        <f>Z18+D7</f>
+        <f t="shared" si="1"/>
         <v>34.474000000000004</v>
       </c>
       <c r="K7" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.0730000000000004</v>
       </c>
       <c r="L7" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.3519999999999994</v>
       </c>
       <c r="M7" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>51.155999999999999</v>
       </c>
       <c r="N7" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>62.820999999999998</v>
       </c>
       <c r="Q7" t="s">
@@ -3458,27 +3458,27 @@
         <v>0.254</v>
       </c>
       <c r="I8" s="2">
-        <f>Y19+C8</f>
+        <f t="shared" si="0"/>
         <v>1.9999999999999997E-2</v>
       </c>
       <c r="J8" s="3">
-        <f>Z19+D8</f>
+        <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
       <c r="K8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="L8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.5E-2</v>
       </c>
       <c r="M8" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.6540000000000001</v>
       </c>
       <c r="N8" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.5549999999999997</v>
       </c>
       <c r="Q8" t="s">
@@ -3512,27 +3512,27 @@
         <v>0.27600000000000002</v>
       </c>
       <c r="I9" s="5">
-        <f>Y20+C9</f>
+        <f t="shared" si="0"/>
         <v>0.56500000000000006</v>
       </c>
       <c r="J9" s="6">
-        <f>Z20+D9</f>
+        <f t="shared" si="1"/>
         <v>0.71699999999999997</v>
       </c>
       <c r="K9" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.19799999999999998</v>
       </c>
       <c r="L9" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.189</v>
       </c>
       <c r="M9" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.46</v>
       </c>
       <c r="N9" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>12.041</v>
       </c>
       <c r="Q9" t="s">
@@ -3566,27 +3566,27 @@
         <v>0.30199999999999999</v>
       </c>
       <c r="I10" s="8">
-        <f>Y21+C10</f>
+        <f t="shared" si="0"/>
         <v>6.3169999999999993</v>
       </c>
       <c r="J10" s="9">
-        <f>Z21+D10</f>
+        <f t="shared" si="1"/>
         <v>7.4109999999999996</v>
       </c>
       <c r="K10" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.3820000000000001</v>
       </c>
       <c r="L10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.4319999999999999</v>
       </c>
       <c r="M10" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>11.901</v>
       </c>
       <c r="N10" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>20.213999999999999</v>
       </c>
       <c r="Q10" t="s">
@@ -3622,27 +3622,27 @@
         <v>0.317</v>
       </c>
       <c r="I11" s="5">
-        <f>Y22+C11</f>
+        <f t="shared" si="0"/>
         <v>0.48099999999999998</v>
       </c>
       <c r="J11" s="6">
-        <f>Z22+D11</f>
+        <f t="shared" si="1"/>
         <v>0.47500000000000003</v>
       </c>
       <c r="K11" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="L11" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.10199999999999999</v>
       </c>
       <c r="M11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.101</v>
       </c>
       <c r="N11" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>11.976000000000001</v>
       </c>
       <c r="Q11" t="s">
@@ -3676,27 +3676,27 @@
         <v>0.34799999999999998</v>
       </c>
       <c r="I12" s="5">
-        <f>Y23+C12</f>
+        <f t="shared" si="0"/>
         <v>4.4240000000000004</v>
       </c>
       <c r="J12" s="6">
-        <f>Z23+D12</f>
+        <f t="shared" si="1"/>
         <v>4.3639999999999999</v>
       </c>
       <c r="K12" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.30300000000000005</v>
       </c>
       <c r="L12" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.38800000000000001</v>
       </c>
       <c r="M12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.827</v>
       </c>
       <c r="N12" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>17.477</v>
       </c>
       <c r="Q12" t="s">
@@ -3730,27 +3730,27 @@
         <v>0.46100000000000002</v>
       </c>
       <c r="I13" s="5">
-        <f>Y24+C13</f>
+        <f t="shared" si="0"/>
         <v>41.741999999999997</v>
       </c>
       <c r="J13" s="6">
-        <f>Z24+D13</f>
+        <f t="shared" si="1"/>
         <v>43.271000000000001</v>
       </c>
       <c r="K13" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.8930000000000002</v>
       </c>
       <c r="L13" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.0489999999999999</v>
       </c>
       <c r="M13" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>57.463999999999999</v>
       </c>
       <c r="N13" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>48.937999999999995</v>
       </c>
       <c r="Q13" t="s">
@@ -3786,27 +3786,27 @@
         <v>0.313</v>
       </c>
       <c r="I14" s="2">
-        <f>Y25+C14</f>
+        <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
       <c r="J14" s="3">
-        <f>Z25+D14</f>
+        <f t="shared" si="1"/>
         <v>0.47500000000000003</v>
       </c>
       <c r="K14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.125</v>
       </c>
       <c r="L14" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.129</v>
       </c>
       <c r="M14" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.1109999999999998</v>
       </c>
       <c r="N14" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>11.75</v>
       </c>
     </row>
@@ -3834,27 +3834,27 @@
         <v>0.29499999999999998</v>
       </c>
       <c r="I15" s="5">
-        <f>Y26+C15</f>
+        <f t="shared" si="0"/>
         <v>4.4069999999999991</v>
       </c>
       <c r="J15" s="6">
-        <f>Z26+D15</f>
+        <f t="shared" si="1"/>
         <v>4.4880000000000004</v>
       </c>
       <c r="K15" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.63900000000000001</v>
       </c>
       <c r="L15" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.64900000000000002</v>
       </c>
       <c r="M15" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7.3620000000000001</v>
       </c>
       <c r="N15" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>16.551000000000002</v>
       </c>
       <c r="Y15" t="s">
@@ -3885,27 +3885,27 @@
         <v>0.45100000000000001</v>
       </c>
       <c r="I16" s="8">
-        <f>Y27+C16</f>
+        <f t="shared" si="0"/>
         <v>43.744</v>
       </c>
       <c r="J16" s="9">
-        <f>Z27+D16</f>
+        <f t="shared" si="1"/>
         <v>44.437999999999995</v>
       </c>
       <c r="K16" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.5060000000000002</v>
       </c>
       <c r="L16" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.2329999999999997</v>
       </c>
       <c r="M16" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>59.597000000000001</v>
       </c>
       <c r="N16" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>47.423999999999999</v>
       </c>
       <c r="Y16" s="3">
@@ -3953,27 +3953,27 @@
         <v>0.34200000000000003</v>
       </c>
       <c r="I17" s="5">
-        <f>Y28+C17</f>
+        <f t="shared" si="0"/>
         <v>0.27800000000000002</v>
       </c>
       <c r="J17" s="6">
-        <f>Z28+D17</f>
+        <f t="shared" si="1"/>
         <v>0.26100000000000001</v>
       </c>
       <c r="K17" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.372</v>
       </c>
       <c r="L17" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.38699999999999996</v>
       </c>
       <c r="M17" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.282</v>
       </c>
       <c r="N17" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>11.39</v>
       </c>
       <c r="Y17" s="6">
@@ -4019,27 +4019,27 @@
         <v>0.40600000000000003</v>
       </c>
       <c r="I18" s="5">
-        <f>Y29+C18</f>
+        <f t="shared" si="0"/>
         <v>1.002</v>
       </c>
       <c r="J18" s="6">
-        <f>Z29+D18</f>
+        <f t="shared" si="1"/>
         <v>0.96699999999999997</v>
       </c>
       <c r="K18" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.3220000000000001</v>
       </c>
       <c r="L18" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.3679999999999999</v>
       </c>
       <c r="M18" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9.2080000000000002</v>
       </c>
       <c r="N18" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>14.229000000000001</v>
       </c>
       <c r="Y18" s="9">
@@ -4085,27 +4085,27 @@
         <v>0.46800000000000003</v>
       </c>
       <c r="I19" s="5">
-        <f>Y30+C19</f>
+        <f t="shared" si="0"/>
         <v>4.2530000000000001</v>
       </c>
       <c r="J19" s="6">
-        <f>Z30+D19</f>
+        <f t="shared" si="1"/>
         <v>4.0170000000000003</v>
       </c>
       <c r="K19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.4030000000000005</v>
       </c>
       <c r="L19" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9270000000000005</v>
       </c>
       <c r="M19" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>34.798000000000002</v>
       </c>
       <c r="N19" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>20.983999999999998</v>
       </c>
       <c r="Y19" s="2">
@@ -4153,27 +4153,27 @@
         <v>1.042</v>
       </c>
       <c r="I20" s="2">
-        <f>Y31+C20</f>
+        <f t="shared" si="0"/>
         <v>2.8159999999999998</v>
       </c>
       <c r="J20" s="3">
-        <f>Z31+D20</f>
+        <f t="shared" si="1"/>
         <v>3.609</v>
       </c>
       <c r="K20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.43700000000000006</v>
       </c>
       <c r="L20" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.49399999999999999</v>
       </c>
       <c r="M20" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.4850000000000003</v>
       </c>
       <c r="N20" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>19.481000000000002</v>
       </c>
       <c r="Y20" s="5">
@@ -4219,27 +4219,27 @@
         <v>1.2410000000000001</v>
       </c>
       <c r="I21" s="5">
-        <f>Y32+C21</f>
+        <f t="shared" si="0"/>
         <v>11.349</v>
       </c>
       <c r="J21" s="6">
-        <f>Z32+D21</f>
+        <f t="shared" si="1"/>
         <v>14.475</v>
       </c>
       <c r="K21" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5209999999999999</v>
       </c>
       <c r="L21" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.649</v>
       </c>
       <c r="M21" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>21.423999999999999</v>
       </c>
       <c r="N21" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>33.4</v>
       </c>
       <c r="Y21" s="8">
@@ -4285,27 +4285,27 @@
         <v>2.3959999999999999</v>
       </c>
       <c r="I22" s="8">
-        <f>Y33+C22</f>
+        <f t="shared" si="0"/>
         <v>23.385000000000002</v>
       </c>
       <c r="J22" s="9">
-        <f>Z33+D22</f>
+        <f t="shared" si="1"/>
         <v>30.937999999999999</v>
       </c>
       <c r="K22" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.01</v>
       </c>
       <c r="L22" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.08</v>
       </c>
       <c r="M22" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>46.259</v>
       </c>
       <c r="N22" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>56.61</v>
       </c>
       <c r="Y22" s="2">
@@ -4353,27 +4353,27 @@
         <v>0.70499999999999996</v>
       </c>
       <c r="I23" s="5">
-        <f>Y34+C23</f>
+        <f t="shared" si="0"/>
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="J23" s="6">
-        <f>Z34+D23</f>
+        <f t="shared" si="1"/>
         <v>3.1E-2</v>
       </c>
       <c r="K23" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="L23" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="M23" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.534</v>
       </c>
       <c r="N23" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10.922000000000001</v>
       </c>
       <c r="Y23" s="5">
@@ -4419,27 +4419,27 @@
         <v>2.302</v>
       </c>
       <c r="I24" s="5">
-        <f>Y35+C24</f>
+        <f t="shared" si="0"/>
         <v>0.71599999999999997</v>
       </c>
       <c r="J24" s="6">
-        <f>Z35+D24</f>
+        <f t="shared" si="1"/>
         <v>0.748</v>
       </c>
       <c r="K24" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.35099999999999998</v>
       </c>
       <c r="L24" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.32399999999999995</v>
       </c>
       <c r="M24" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.1379999999999999</v>
       </c>
       <c r="N24" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>21.248000000000001</v>
       </c>
       <c r="Y24" s="8">
@@ -4485,27 +4485,27 @@
         <v>2.254</v>
       </c>
       <c r="I25" s="5">
-        <f>Y36+C25</f>
+        <f t="shared" si="0"/>
         <v>13.019</v>
       </c>
       <c r="J25" s="6">
-        <f>Z36+D25</f>
+        <f t="shared" si="1"/>
         <v>13.673</v>
       </c>
       <c r="K25" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.8759999999999999</v>
       </c>
       <c r="L25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.625</v>
       </c>
       <c r="M25" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>43.695</v>
       </c>
       <c r="N25" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>45.745999999999995</v>
       </c>
       <c r="P25" t="s">
@@ -4556,27 +4556,27 @@
         <v>0.66200000000000003</v>
       </c>
       <c r="I26" s="2">
-        <f>Y37+C26</f>
+        <f t="shared" si="0"/>
         <v>0.22600000000000001</v>
       </c>
       <c r="J26" s="3">
-        <f>Z37+D26</f>
+        <f t="shared" si="1"/>
         <v>0.26700000000000002</v>
       </c>
       <c r="K26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.23099999999999998</v>
       </c>
       <c r="L26" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.20699999999999999</v>
       </c>
       <c r="M26" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.6120000000000001</v>
       </c>
       <c r="N26" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>13.494000000000002</v>
       </c>
       <c r="O26" t="s">
@@ -4625,27 +4625,27 @@
         <v>0.96899999999999997</v>
       </c>
       <c r="I27" s="5">
-        <f>Y38+C27</f>
+        <f t="shared" si="0"/>
         <v>3.8610000000000002</v>
       </c>
       <c r="J27" s="6">
-        <f>Z38+D27</f>
+        <f t="shared" si="1"/>
         <v>3.1539999999999999</v>
       </c>
       <c r="K27" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.4379999999999999</v>
       </c>
       <c r="L27" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.89</v>
       </c>
       <c r="M27" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>16.745999999999999</v>
       </c>
       <c r="N27" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>23.752000000000002</v>
       </c>
       <c r="Y27" s="9">
@@ -4691,27 +4691,27 @@
         <v>0.97099999999999997</v>
       </c>
       <c r="I28" s="8">
-        <f>Y39+C28</f>
+        <f t="shared" si="0"/>
         <v>16.771000000000001</v>
       </c>
       <c r="J28" s="9">
-        <f>Z39+D28</f>
+        <f t="shared" si="1"/>
         <v>14.267000000000001</v>
       </c>
       <c r="K28" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.5279999999999996</v>
       </c>
       <c r="L28" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.222</v>
       </c>
       <c r="M28" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>68.26100000000001</v>
       </c>
       <c r="N28" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>47.76</v>
       </c>
       <c r="Y28" s="3">
@@ -4759,27 +4759,27 @@
         <v>0.63100000000000001</v>
       </c>
       <c r="I29" s="5">
-        <f>Y40+C29</f>
+        <f t="shared" si="0"/>
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="J29" s="6">
-        <f>Z40+D29</f>
+        <f t="shared" si="1"/>
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="K29" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.13300000000000001</v>
       </c>
       <c r="L29" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.16300000000000001</v>
       </c>
       <c r="M29" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.2949999999999999</v>
       </c>
       <c r="N29" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>14.332000000000001</v>
       </c>
       <c r="Y29" s="18">
@@ -4825,27 +4825,27 @@
         <v>2.7549999999999999</v>
       </c>
       <c r="I30" s="5">
-        <f>Y41+C30</f>
+        <f t="shared" si="0"/>
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="J30" s="6">
-        <f>Z41+D30</f>
+        <f t="shared" si="1"/>
         <v>4.5000000000000005E-2</v>
       </c>
       <c r="K30" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.10199999999999999</v>
       </c>
       <c r="L30" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.159</v>
       </c>
       <c r="M30" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>16.53</v>
       </c>
       <c r="N30" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>27.875</v>
       </c>
       <c r="Y30" s="9">
@@ -4891,27 +4891,27 @@
         <v>6.5720000000000001</v>
       </c>
       <c r="I31" s="5">
-        <f>Y42+C31</f>
+        <f t="shared" si="0"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="J31" s="6">
-        <f>Z42+D31</f>
+        <f t="shared" si="1"/>
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="K31" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.106</v>
       </c>
       <c r="L31" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.16900000000000001</v>
       </c>
       <c r="M31" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>43.007999999999996</v>
       </c>
       <c r="N31" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>51.373000000000005</v>
       </c>
       <c r="Y31" s="3">
@@ -4959,27 +4959,27 @@
         <v>0.38300000000000001</v>
       </c>
       <c r="I32" s="2">
-        <f>Y43+C32</f>
+        <f t="shared" si="0"/>
         <v>7.3740000000000006</v>
       </c>
       <c r="J32" s="3">
-        <f>Z43+D32</f>
+        <f t="shared" si="1"/>
         <v>14.54</v>
       </c>
       <c r="K32" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.79600000000000004</v>
       </c>
       <c r="L32" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.2529999999999997</v>
       </c>
       <c r="M32" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12.774000000000001</v>
       </c>
       <c r="N32" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>20.701000000000001</v>
       </c>
       <c r="Y32" s="18">
@@ -5025,27 +5025,27 @@
         <v>0.52300000000000002</v>
       </c>
       <c r="I33" s="5">
-        <f>Y44+C33</f>
+        <f t="shared" si="0"/>
         <v>14.446999999999999</v>
       </c>
       <c r="J33" s="6">
-        <f>Z44+D33</f>
+        <f t="shared" si="1"/>
         <v>27.756</v>
       </c>
       <c r="K33" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5069999999999999</v>
       </c>
       <c r="L33" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.7169999999999996</v>
       </c>
       <c r="M33" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>26.698</v>
       </c>
       <c r="N33" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>27.24</v>
       </c>
       <c r="Y33" s="9">
@@ -5091,27 +5091,27 @@
         <v>2.4329999999999998</v>
       </c>
       <c r="I34" s="8">
-        <f>Y45+C34</f>
+        <f t="shared" si="0"/>
         <v>28.444000000000003</v>
       </c>
       <c r="J34" s="9">
-        <f>Z45+D34</f>
+        <f t="shared" si="1"/>
         <v>59.353999999999999</v>
       </c>
       <c r="K34" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.7930000000000001</v>
       </c>
       <c r="L34" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>10.957000000000001</v>
       </c>
       <c r="M34" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>52.117000000000004</v>
       </c>
       <c r="N34" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>40.795000000000002</v>
       </c>
       <c r="Y34" s="3">
@@ -5363,7 +5363,7 @@
     <hyperlink ref="R9" r:id="rId6"/>
     <hyperlink ref="R10" r:id="rId7" location="Python:_Simple_Backtracking_Solution"/>
     <hyperlink ref="R11" r:id="rId8" location="Python"/>
-    <hyperlink ref="R13" r:id="rId9" location="Python" display="https://rosettacode.org/wiki/100_prisoners - Python"/>
+    <hyperlink ref="R13" r:id="rId9" location="Python"/>
     <hyperlink ref="R12" r:id="rId10" location="Python"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>